<commit_message>
BM-1575 implement state tax sql write out
</commit_message>
<xml_diff>
--- a/state_tax_importer/sample_state_tax_input_excel.xlsx
+++ b/state_tax_importer/sample_state_tax_input_excel.xlsx
@@ -56,7 +56,7 @@
     <t>TP1-EMP-00001</t>
   </si>
   <si>
-    <t>Simon</t>
+    <t>Simon3</t>
   </si>
   <si>
     <t>AA</t>
@@ -194,7 +194,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>